<commit_message>
Deployed 2d4e9d7 to dev with MkDocs 1.6.1 and mike 2.1.3
</commit_message>
<xml_diff>
--- a/dev/fhir-ig/StructureDefinition-onconova-Karnofsky-performance-status.xlsx
+++ b/dev/fhir-ig/StructureDefinition-onconova-Karnofsky-performance-status.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-29T08:09:08+00:00</t>
+    <t>2025-10-09T11:26:42+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -3324,7 +3324,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" hidden="true">
+    <row r="14">
       <c r="A14" t="s" s="2">
         <v>172</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" hidden="true">
+    <row r="16">
       <c r="A16" t="s" s="2">
         <v>198</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" hidden="true">
+    <row r="17">
       <c r="A17" t="s" s="2">
         <v>203</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="18" hidden="true">
+    <row r="18">
       <c r="A18" t="s" s="2">
         <v>218</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" hidden="true">
+    <row r="21">
       <c r="A21" t="s" s="2">
         <v>241</v>
       </c>
@@ -4536,7 +4536,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" hidden="true">
+    <row r="24">
       <c r="A24" t="s" s="2">
         <v>267</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="25" hidden="true">
+    <row r="25">
       <c r="A25" t="s" s="2">
         <v>279</v>
       </c>
@@ -4780,7 +4780,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" hidden="true">
+    <row r="26">
       <c r="A26" t="s" s="2">
         <v>286</v>
       </c>
@@ -8038,12 +8038,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AP52">
-    <filterColumn colId="6">
+    <filterColumn colId="7">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
-    <filterColumn colId="26">
+    <filterColumn colId="27">
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>

</xml_diff>